<commit_message>
made comparisons between standard,with numbers, and orginal countin, in different files formats, added exporting of processed files
</commit_message>
<xml_diff>
--- a/Reproducible_example_EUR-Lex.xlsx
+++ b/Reproducible_example_EUR-Lex.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c0ac04fbadbefb8/SDG/Policy-Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{914D7AAD-8CE1-4784-A40E-36998313096D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FC3564AD-33AF-4780-9ED3-5661EBBBAED7}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{914D7AAD-8CE1-4784-A40E-36998313096D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EC266CF2-5276-4302-A0AB-C02E8E288C6E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60E67003-CA50-4859-8748-6AEC2013F6E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="91">
   <si>
     <t>Path</t>
   </si>
@@ -78,12 +78,6 @@
     <t>52019DC0640</t>
   </si>
   <si>
-    <t>52019DC0641</t>
-  </si>
-  <si>
-    <t>52019DC0642</t>
-  </si>
-  <si>
     <t>https://eur-lex.europa.eu/legal-content/EN/TXT/HTML/?uri=CELEX:52019DC0640&amp;qid=1611589407263&amp;from=EN</t>
   </si>
   <si>
@@ -150,18 +144,6 @@
     <t>11th_European_Development_Fund_covering_the_period_2014-2018</t>
   </si>
   <si>
-    <t>52017DC0160</t>
-  </si>
-  <si>
-    <t>52017DC0161</t>
-  </si>
-  <si>
-    <t>52017SC0124</t>
-  </si>
-  <si>
-    <t>52017SC0125</t>
-  </si>
-  <si>
     <t>52020DC0667</t>
   </si>
   <si>
@@ -222,21 +204,6 @@
     <t>52020DC0381</t>
   </si>
   <si>
-    <t>52020DC0382</t>
-  </si>
-  <si>
-    <t>52020DC0383</t>
-  </si>
-  <si>
-    <t>https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.02/DOC_1&amp;format=PDF;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.02/DOC_2&amp;format=PDF;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.02/DOC_3&amp;format=PDF</t>
-  </si>
-  <si>
-    <t>https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.01/DOC_1&amp;format=DOC;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.01/DOC_2&amp;format=DOC;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.01/DOC_3&amp;format=DOC</t>
-  </si>
-  <si>
-    <t>https://eur-lex.europa.eu/legal-content/FR/TXT/HTML/?uri=CELEX:52020DC0620&amp;from=EN</t>
-  </si>
-  <si>
     <t>https://eur-lex.europa.eu/legal-content/EN/TXT/PDF/?uri=CELEX:52020DC0152&amp;rid=5</t>
   </si>
   <si>
@@ -249,12 +216,6 @@
     <t>52020DC0152</t>
   </si>
   <si>
-    <t>52020DC0153</t>
-  </si>
-  <si>
-    <t>52020DC0154</t>
-  </si>
-  <si>
     <t>https://eur-lex.europa.eu/resource.html?uri=cellar:ea0f9f73-9ab2-11ea-9d2d-01aa75ed71a1.0001.02/DOC_1&amp;format=PDF;https://eur-lex.europa.eu/resource.html?uri=cellar:ea0f9f73-9ab2-11ea-9d2d-01aa75ed71a1.0001.02/DOC_2&amp;format=PDF</t>
   </si>
   <si>
@@ -288,9 +249,6 @@
     <t>https://eur-lex.europa.eu/resource.html?uri=cellar:749e04bb-f8c5-11ea-991b-01aa75ed71a1.0001.02/DOC_1&amp;format=PDF;https://eur-lex.europa.eu/resource.html?uri=cellar:749e04bb-f8c5-11ea-991b-01aa75ed71a1.0001.02/DOC_2&amp;format=PDF</t>
   </si>
   <si>
-    <t>https://eur-lex.europa.eu/legal-content/EN/TXT/DOC/?uri=CELEX:52020DC0667&amp;qid=1611592111695&amp;from=EN</t>
-  </si>
-  <si>
     <t>https://eur-lex.europa.eu/legal-content/EN/TXT/DOC/?uri=CELEX:52020SC0225&amp;qid=1611592111695&amp;from=EN</t>
   </si>
   <si>
@@ -321,7 +279,34 @@
     <t>https://eur-lex.europa.eu/legal-content/EN/TXT/PDF/?uri=CELEX:52020SC0251&amp;qid=1611592111695&amp;from=EN</t>
   </si>
   <si>
-    <t>https://eur-lex.europa.eu/legal-content/EN/TXT/PDF/?uri=CELEX:52020DC0667&amp;qid=1611592111695&amp;from=EN</t>
+    <t>European_Climate_Pact</t>
+  </si>
+  <si>
+    <t>52020DC0788</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/legal-content/EN/TXT/HTML/?uri=CELEX:52020DC0788&amp;qid=1612879270611&amp;from=EN</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/legal-content/EN/TXT/DOC/?uri=CELEX:52020DC0788&amp;qid=1612879270611&amp;from=EN</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/legal-content/EN/TXT/PDF/?uri=CELEX:52020DC0788&amp;qid=1612879270611&amp;from=EN</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/legal-content/EN/TXT/HTML/?uri=CELEX:52020DC0620&amp;from=EN</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0001.01/DOC_1&amp;format=DOC;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0001.01/DOC_2&amp;format=DOC;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0001.01/DOC_3&amp;format=DOC</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0001.02/DOC_1&amp;format=PDF;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0001.02/DOC_2&amp;format=PDF;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0001.02/DOC_3&amp;format=PDF</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/resource.html?uri=cellar:f815479a-0f01-11eb-bc07-01aa75ed71a1.0003.01/DOC_1&amp;format=DOC;https://eur-lex.europa.eu/resource.html?uri=cellar:f815479a-0f01-11eb-bc07-01aa75ed71a1.0003.01/DOC_2&amp;format=DOC</t>
+  </si>
+  <si>
+    <t>https://eur-lex.europa.eu/resource.html?uri=cellar:f815479a-0f01-11eb-bc07-01aa75ed71a1.0003.02/DOC_1&amp;format=PDF;https://eur-lex.europa.eu/resource.html?uri=cellar:f815479a-0f01-11eb-bc07-01aa75ed71a1.0003.02/DOC_2&amp;format=PDF</t>
   </si>
 </sst>
 </file>
@@ -372,10 +357,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -691,16 +677,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45241D01-CD59-43BA-B4CC-6F73673807B4}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="110.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="110.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -709,7 +695,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C1" t="s">
@@ -726,283 +712,283 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>36</v>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>37</v>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
+      <c r="B9" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>7</v>
+      <c r="B11" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
-        <v>7</v>
+      <c r="B12" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
-        <v>7</v>
+      <c r="B13" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
-        <v>7</v>
+      <c r="B14" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
-        <v>7</v>
+      <c r="B15" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
-        <v>7</v>
+      <c r="B16" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -1015,11 +1001,11 @@
       <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -1032,617 +1018,669 @@
       <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
-      <c r="B29" t="s">
-        <v>8</v>
+      <c r="B29" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>4</v>
       </c>
-      <c r="B30" t="s">
-        <v>8</v>
+      <c r="B30" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
-      <c r="B31" t="s">
-        <v>8</v>
+      <c r="B31" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="B32" t="s">
-        <v>8</v>
+      <c r="B32" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
-      <c r="B33" t="s">
-        <v>8</v>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
-      <c r="B34" t="s">
-        <v>8</v>
+      <c r="B34" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
-      <c r="B35" t="s">
-        <v>8</v>
+      <c r="B35" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B36" t="s">
-        <v>8</v>
+      <c r="B36" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
-      <c r="B37" t="s">
-        <v>8</v>
+      <c r="B37" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" t="s">
-        <v>8</v>
+      <c r="B38" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>4</v>
       </c>
-      <c r="B39" t="s">
-        <v>8</v>
+      <c r="B39" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40" t="s">
-        <v>8</v>
+      <c r="B40" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B41" t="s">
-        <v>9</v>
+      <c r="B41" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D41" t="s">
         <v>10</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" t="s">
-        <v>9</v>
+      <c r="B42" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>18</v>
+      <c r="E42" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>4</v>
       </c>
-      <c r="B43" t="s">
-        <v>9</v>
+      <c r="B43" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>17</v>
+      <c r="E43" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>4</v>
       </c>
-      <c r="B44" t="s">
-        <v>55</v>
+      <c r="B44" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="D44" t="s">
         <v>10</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>4</v>
       </c>
-      <c r="B45" t="s">
-        <v>55</v>
+      <c r="B45" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" t="s">
-        <v>55</v>
+      <c r="B46" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>4</v>
       </c>
-      <c r="B47" t="s">
-        <v>57</v>
+      <c r="B47" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="D47" t="s">
         <v>10</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>4</v>
       </c>
-      <c r="B48" t="s">
-        <v>58</v>
+      <c r="B48" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
-      <c r="B49" t="s">
-        <v>59</v>
+      <c r="B49" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="D49" t="s">
         <v>12</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
-      <c r="B50" t="s">
-        <v>56</v>
+      <c r="B50" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D50" t="s">
         <v>10</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
-      <c r="B51" t="s">
-        <v>56</v>
+      <c r="B51" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4</v>
       </c>
-      <c r="B52" t="s">
-        <v>56</v>
+      <c r="B52" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E55">
+    <sortCondition ref="B2:B55"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{C83F7192-CA50-499B-9400-07EC5F4D3928}"/>
-    <hyperlink ref="E10" r:id="rId2" xr:uid="{BEA81054-AC1E-4725-8533-76804FBC40D0}"/>
-    <hyperlink ref="E12" r:id="rId3" xr:uid="{04D064A4-1A76-4312-AC60-9DF5E2E7D9ED}"/>
-    <hyperlink ref="E13" r:id="rId4" xr:uid="{5394A14B-67C3-473B-B7F2-87536E81BF85}"/>
-    <hyperlink ref="E15" r:id="rId5" xr:uid="{01054157-E9AE-43D5-B382-015DD2107372}"/>
-    <hyperlink ref="E16" r:id="rId6" xr:uid="{343A6866-83CE-4521-B46A-E84F5DA3EF58}"/>
-    <hyperlink ref="E18" r:id="rId7" xr:uid="{DDA8E0A4-9E64-4BFC-9AF4-8376B14AA389}"/>
-    <hyperlink ref="E19" r:id="rId8" xr:uid="{EC19711F-C878-4ACA-B612-9B2FE54EED86}"/>
-    <hyperlink ref="E21" r:id="rId9" xr:uid="{EA1F8DB2-9DBD-428B-941C-9BF9886F5590}"/>
-    <hyperlink ref="E22" r:id="rId10" xr:uid="{13619FBC-16BF-4505-B4DF-28A86BAE16F4}"/>
-    <hyperlink ref="E24" r:id="rId11" xr:uid="{E6A6FC64-23F9-4FEB-B62D-E3CC73C69E4D}"/>
-    <hyperlink ref="E25" r:id="rId12" xr:uid="{0EA0AC52-60CA-44D3-A015-17DB414B87CA}"/>
-    <hyperlink ref="E27" r:id="rId13" xr:uid="{77D74237-F182-4EAE-A1BC-74C8E37F39C4}"/>
-    <hyperlink ref="E28" r:id="rId14" xr:uid="{15933F95-F5E5-4913-98D0-2E318D465729}"/>
-    <hyperlink ref="E2" r:id="rId15" xr:uid="{656B9EB3-CDEA-46F3-A723-E130E9DD5E64}"/>
-    <hyperlink ref="E3" r:id="rId16" xr:uid="{ED4D9ECE-F6A7-43C5-AD39-70D400AC343A}"/>
-    <hyperlink ref="E4" r:id="rId17" xr:uid="{8A5B369D-B86A-404B-BD41-86972EA5168A}"/>
-    <hyperlink ref="E5" r:id="rId18" xr:uid="{8CB5D87B-3A96-40D5-9961-3A31020953E6}"/>
-    <hyperlink ref="E6" r:id="rId19" xr:uid="{B6A2E231-F251-4D13-B974-512BCBD661F1}"/>
-    <hyperlink ref="E7" r:id="rId20" xr:uid="{13A12F67-D584-44C6-ABF3-187B287D914A}"/>
-    <hyperlink ref="E8" r:id="rId21" xr:uid="{1E5446FA-B44A-4905-B616-E63EC5B35F81}"/>
-    <hyperlink ref="E11" r:id="rId22" xr:uid="{C0DD5958-A976-4B6C-A330-CEAEEE24D586}"/>
-    <hyperlink ref="E14" r:id="rId23" xr:uid="{5DCB8114-B971-4AB6-A9E8-14E25A2DE3A4}"/>
-    <hyperlink ref="E17" r:id="rId24" xr:uid="{9EBB073C-4762-4100-8DC7-81B30F7A7156}"/>
-    <hyperlink ref="E20" r:id="rId25" xr:uid="{1FCA4FDC-B697-44D4-836D-14B33CFC1714}"/>
-    <hyperlink ref="E23" r:id="rId26" xr:uid="{AA061AC4-E2B0-4846-B314-FE82361E9DD3}"/>
-    <hyperlink ref="E26" r:id="rId27" xr:uid="{C791D254-0EE1-47B8-9645-523FCDFB3A96}"/>
-    <hyperlink ref="E29" r:id="rId28" xr:uid="{90EC3825-593C-4881-AA18-E3248F130F09}"/>
-    <hyperlink ref="E30" r:id="rId29" xr:uid="{7590E040-C30C-4579-ACD0-22D7BE0D363C}"/>
-    <hyperlink ref="E31" r:id="rId30" xr:uid="{5261F755-B926-435C-95BC-E842D94FFCE1}"/>
-    <hyperlink ref="E32" r:id="rId31" xr:uid="{9136F62E-ADC4-4882-AC9C-E0C2AEC8DBDB}"/>
-    <hyperlink ref="E33" r:id="rId32" xr:uid="{45B007EE-5005-4E13-912A-028633AF87BD}"/>
-    <hyperlink ref="E34" r:id="rId33" xr:uid="{9512BB09-8C6D-4815-93D2-169BA23E8E5C}"/>
-    <hyperlink ref="E35" r:id="rId34" xr:uid="{567A68FC-1ACF-41EE-BD1D-462E722A94A5}"/>
-    <hyperlink ref="E36" r:id="rId35" xr:uid="{D31EE1BE-2DA8-4138-9BEA-A28AFE8DC8A6}"/>
-    <hyperlink ref="E37" r:id="rId36" xr:uid="{06011B5D-F7DF-4F47-B062-1056CE972CF2}"/>
-    <hyperlink ref="E38" r:id="rId37" xr:uid="{E911DC96-B662-437F-A039-37A124CD4BE4}"/>
-    <hyperlink ref="E39" r:id="rId38" xr:uid="{B2C6F0EA-22B0-4C2E-AC52-9E41F395FD67}"/>
-    <hyperlink ref="E40" r:id="rId39" xr:uid="{DA8FEFAE-5810-481D-A09C-F763651D2ABC}"/>
-    <hyperlink ref="E41" r:id="rId40" xr:uid="{B53F0F2B-8AD3-4720-BC6C-8DF403DF6445}"/>
-    <hyperlink ref="E42" r:id="rId41" xr:uid="{F3A5EDB4-E83B-40E7-9393-B54F787B51AC}"/>
-    <hyperlink ref="E43" r:id="rId42" xr:uid="{9B970989-7A09-44C2-B225-CB2183BE904F}"/>
-    <hyperlink ref="E44" r:id="rId43" xr:uid="{0148AD81-EFA2-4C85-AA29-79307F64B2E7}"/>
-    <hyperlink ref="E45" r:id="rId44" xr:uid="{D8532FDD-F17F-43F0-9C2D-058C013AF723}"/>
-    <hyperlink ref="E46" r:id="rId45" xr:uid="{0D0892A9-451D-4E0F-AABB-FFFAC96CA4CC}"/>
-    <hyperlink ref="E47" r:id="rId46" xr:uid="{3CC91FB5-E5B0-4361-9059-A0DE2BF98851}"/>
-    <hyperlink ref="E48" r:id="rId47" xr:uid="{FD13ECA9-26F8-446D-A3D2-7444DF734C11}"/>
-    <hyperlink ref="E49" r:id="rId48" xr:uid="{B10AA6E7-277F-49C5-878D-C3FAB8A801EF}"/>
-    <hyperlink ref="E50" r:id="rId49" xr:uid="{DE90654D-885B-46BC-A2E1-B99613639ECA}"/>
-    <hyperlink ref="E51" r:id="rId50" display="https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.01/DOC_1&amp;format=DOC;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.01/DOC_2&amp;format=DOC;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.01/DOC_3&amp;format=DOC" xr:uid="{F7940D5F-38E9-4360-B902-E665C43535AE}"/>
-    <hyperlink ref="E52" r:id="rId51" display="https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.02/DOC_1&amp;format=PDF;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.02/DOC_2&amp;format=PDF;https://eur-lex.europa.eu/resource.html?uri=cellar:9a007e7e-08ad-11eb-a511-01aa75ed71a1.0012.02/DOC_3&amp;format=PDF" xr:uid="{3CD732C8-093A-40F6-8357-23C6B48D5896}"/>
+    <hyperlink ref="E21" r:id="rId1" xr:uid="{04D064A4-1A76-4312-AC60-9DF5E2E7D9ED}"/>
+    <hyperlink ref="E22" r:id="rId2" xr:uid="{5394A14B-67C3-473B-B7F2-87536E81BF85}"/>
+    <hyperlink ref="E24" r:id="rId3" xr:uid="{01054157-E9AE-43D5-B382-015DD2107372}"/>
+    <hyperlink ref="E25" r:id="rId4" xr:uid="{343A6866-83CE-4521-B46A-E84F5DA3EF58}"/>
+    <hyperlink ref="E27" r:id="rId5" xr:uid="{DDA8E0A4-9E64-4BFC-9AF4-8376B14AA389}"/>
+    <hyperlink ref="E28" r:id="rId6" xr:uid="{EC19711F-C878-4ACA-B612-9B2FE54EED86}"/>
+    <hyperlink ref="E30" r:id="rId7" xr:uid="{EA1F8DB2-9DBD-428B-941C-9BF9886F5590}"/>
+    <hyperlink ref="E31" r:id="rId8" xr:uid="{13619FBC-16BF-4505-B4DF-28A86BAE16F4}"/>
+    <hyperlink ref="E33" r:id="rId9" xr:uid="{E6A6FC64-23F9-4FEB-B62D-E3CC73C69E4D}"/>
+    <hyperlink ref="E34" r:id="rId10" xr:uid="{0EA0AC52-60CA-44D3-A015-17DB414B87CA}"/>
+    <hyperlink ref="E36" r:id="rId11" xr:uid="{77D74237-F182-4EAE-A1BC-74C8E37F39C4}"/>
+    <hyperlink ref="E37" r:id="rId12" xr:uid="{15933F95-F5E5-4913-98D0-2E318D465729}"/>
+    <hyperlink ref="E2" r:id="rId13" xr:uid="{656B9EB3-CDEA-46F3-A723-E130E9DD5E64}"/>
+    <hyperlink ref="E3" r:id="rId14" xr:uid="{ED4D9ECE-F6A7-43C5-AD39-70D400AC343A}"/>
+    <hyperlink ref="E5" r:id="rId15" xr:uid="{8A5B369D-B86A-404B-BD41-86972EA5168A}"/>
+    <hyperlink ref="E4" r:id="rId16" xr:uid="{8CB5D87B-3A96-40D5-9961-3A31020953E6}"/>
+    <hyperlink ref="E6" r:id="rId17" xr:uid="{B6A2E231-F251-4D13-B974-512BCBD661F1}"/>
+    <hyperlink ref="E7" r:id="rId18" xr:uid="{13A12F67-D584-44C6-ABF3-187B287D914A}"/>
+    <hyperlink ref="E17" r:id="rId19" xr:uid="{1E5446FA-B44A-4905-B616-E63EC5B35F81}"/>
+    <hyperlink ref="E20" r:id="rId20" xr:uid="{C0DD5958-A976-4B6C-A330-CEAEEE24D586}"/>
+    <hyperlink ref="E23" r:id="rId21" xr:uid="{5DCB8114-B971-4AB6-A9E8-14E25A2DE3A4}"/>
+    <hyperlink ref="E26" r:id="rId22" xr:uid="{9EBB073C-4762-4100-8DC7-81B30F7A7156}"/>
+    <hyperlink ref="E29" r:id="rId23" xr:uid="{1FCA4FDC-B697-44D4-836D-14B33CFC1714}"/>
+    <hyperlink ref="E32" r:id="rId24" xr:uid="{AA061AC4-E2B0-4846-B314-FE82361E9DD3}"/>
+    <hyperlink ref="E35" r:id="rId25" xr:uid="{C791D254-0EE1-47B8-9645-523FCDFB3A96}"/>
+    <hyperlink ref="E41" r:id="rId26" xr:uid="{90EC3825-593C-4881-AA18-E3248F130F09}"/>
+    <hyperlink ref="E42" r:id="rId27" xr:uid="{7590E040-C30C-4579-ACD0-22D7BE0D363C}"/>
+    <hyperlink ref="E43" r:id="rId28" xr:uid="{5261F755-B926-435C-95BC-E842D94FFCE1}"/>
+    <hyperlink ref="E44" r:id="rId29" xr:uid="{9136F62E-ADC4-4882-AC9C-E0C2AEC8DBDB}"/>
+    <hyperlink ref="E45" r:id="rId30" xr:uid="{45B007EE-5005-4E13-912A-028633AF87BD}"/>
+    <hyperlink ref="E46" r:id="rId31" xr:uid="{9512BB09-8C6D-4815-93D2-169BA23E8E5C}"/>
+    <hyperlink ref="E47" r:id="rId32" xr:uid="{567A68FC-1ACF-41EE-BD1D-462E722A94A5}"/>
+    <hyperlink ref="E48" r:id="rId33" xr:uid="{D31EE1BE-2DA8-4138-9BEA-A28AFE8DC8A6}"/>
+    <hyperlink ref="E49" r:id="rId34" xr:uid="{06011B5D-F7DF-4F47-B062-1056CE972CF2}"/>
+    <hyperlink ref="E50" r:id="rId35" xr:uid="{E911DC96-B662-437F-A039-37A124CD4BE4}"/>
+    <hyperlink ref="E51" r:id="rId36" xr:uid="{B2C6F0EA-22B0-4C2E-AC52-9E41F395FD67}"/>
+    <hyperlink ref="E52" r:id="rId37" xr:uid="{DA8FEFAE-5810-481D-A09C-F763651D2ABC}"/>
+    <hyperlink ref="E53" r:id="rId38" xr:uid="{B53F0F2B-8AD3-4720-BC6C-8DF403DF6445}"/>
+    <hyperlink ref="E54" r:id="rId39" xr:uid="{F3A5EDB4-E83B-40E7-9393-B54F787B51AC}"/>
+    <hyperlink ref="E55" r:id="rId40" xr:uid="{9B970989-7A09-44C2-B225-CB2183BE904F}"/>
+    <hyperlink ref="E8" r:id="rId41" xr:uid="{0148AD81-EFA2-4C85-AA29-79307F64B2E7}"/>
+    <hyperlink ref="E9" r:id="rId42" xr:uid="{D8532FDD-F17F-43F0-9C2D-058C013AF723}"/>
+    <hyperlink ref="E10" r:id="rId43" xr:uid="{0D0892A9-451D-4E0F-AABB-FFFAC96CA4CC}"/>
+    <hyperlink ref="E14" r:id="rId44" xr:uid="{3CC91FB5-E5B0-4361-9059-A0DE2BF98851}"/>
+    <hyperlink ref="E15" r:id="rId45" xr:uid="{FD13ECA9-26F8-446D-A3D2-7444DF734C11}"/>
+    <hyperlink ref="E16" r:id="rId46" xr:uid="{B10AA6E7-277F-49C5-878D-C3FAB8A801EF}"/>
+    <hyperlink ref="E38" r:id="rId47" xr:uid="{64D10567-D1F7-4037-A458-40347D87AC82}"/>
+    <hyperlink ref="E39" r:id="rId48" xr:uid="{68308E46-9BFB-4F35-BDA0-5DCEB88823B9}"/>
+    <hyperlink ref="E40" r:id="rId49" xr:uid="{7FBA8BF5-6D1B-4623-8BC3-185A4DA0BFE2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>